<commit_message>
aktualizace algoritmu výměna barev, zatím rozpracováno
</commit_message>
<xml_diff>
--- a/linky_layouts/Kopie - barvovka.xlsx
+++ b/linky_layouts/Kopie - barvovka.xlsx
@@ -11,12 +11,12 @@
     <sheet name="List2" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Barvovka</t>
   </si>
@@ -30,21 +30,9 @@
     <t>Výměna barev</t>
   </si>
   <si>
-    <t>88s</t>
-  </si>
-  <si>
-    <t>254s</t>
-  </si>
-  <si>
     <t>Base</t>
   </si>
   <si>
-    <t>40s</t>
-  </si>
-  <si>
-    <t>100s</t>
-  </si>
-  <si>
     <t>Clear</t>
   </si>
   <si>
@@ -52,6 +40,18 @@
   </si>
   <si>
     <t xml:space="preserve">Ke každé výměně barev je nutné ještě připočítat 8-12s kvůli vyschnutí aplikátoru. </t>
+  </si>
+  <si>
+    <t>Čištění [s]</t>
+  </si>
+  <si>
+    <t>Výměna barev [s]</t>
+  </si>
+  <si>
+    <t>Vyschnutí aplikátoru  [s]</t>
+  </si>
+  <si>
+    <t>Výměna celkem  [s]</t>
   </si>
 </sst>
 </file>
@@ -400,44 +400,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>88</v>
+      </c>
+      <c r="C4">
+        <v>254</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <f>C4+D4</f>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -446,36 +461,50 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E5:E10" si="0">C7+D7</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>88</v>
+      </c>
+      <c r="C10">
+        <v>254</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>